<commit_message>
added my own version of random walks
</commit_message>
<xml_diff>
--- a/algorithms_results/Yardens_results/Apriori_subgroups_results_delta_10000_0.xlsx
+++ b/algorithms_results/Yardens_results/Apriori_subgroups_results_delta_10000_0.xlsx
@@ -790,7 +790,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -806,7 +806,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -838,7 +838,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -870,7 +870,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -886,7 +886,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -902,7 +902,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -934,7 +934,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -966,7 +966,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1014,7 +1014,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'Country': '2'}</t>
+          <t>{'Country': '2', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1046,7 +1046,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>{'GDP': '2', 'Country': '2'}</t>
+          <t>{'Country': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1078,7 +1078,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1094,7 +1094,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2'}</t>
+          <t>{'UndergradMajor': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1110,7 +1110,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1'}</t>
+          <t>{'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1126,7 +1126,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HoursComputer': '2'}</t>
+          <t>{'HoursComputer': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1142,7 +1142,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1174,7 +1174,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1206,7 +1206,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'Student': '1'}</t>
+          <t>{'Student': '1', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1222,7 +1222,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1238,7 +1238,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1254,7 +1254,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1'}</t>
+          <t>{'GDP': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1270,7 +1270,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GINI': '1'}</t>
+          <t>{'GINI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1286,7 +1286,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GINI': '2'}</t>
+          <t>{'GINI': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1318,7 +1318,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1334,7 +1334,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1350,7 +1350,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'UndergradMajor': '2'}</t>
+          <t>{'UndergradMajor': '2', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1366,7 +1366,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'UndergradMajor': '2'}</t>
+          <t>{'UndergradMajor': '2', 'HoursComputer': '2'}</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1382,7 +1382,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2'}</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1398,7 +1398,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2'}</t>
+          <t>{'UndergradMajor': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1446,7 +1446,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'HoursComputer': '2'}</t>
+          <t>{'HoursComputer': '2', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1462,7 +1462,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1494,7 +1494,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1510,7 +1510,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1526,7 +1526,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2'}</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1542,7 +1542,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HoursComputer': '2'}</t>
+          <t>{'HoursComputer': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1590,7 +1590,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1606,7 +1606,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2'}</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1622,7 +1622,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>{'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1638,7 +1638,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3'}</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1654,7 +1654,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1670,7 +1670,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1686,7 +1686,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>{'GINI': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GINI': '2'}</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1702,7 +1702,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1734,7 +1734,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1750,7 +1750,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1782,7 +1782,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GINI': '1'}</t>
+          <t>{'GINI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1798,7 +1798,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GINI': '2'}</t>
+          <t>{'GINI': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1814,7 +1814,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>{'Continent': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1846,7 +1846,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1862,7 +1862,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1926,7 +1926,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2'}</t>
+          <t>{'GINI': '2', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1942,7 +1942,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1974,7 +1974,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>{'GDP': '2', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -2022,7 +2022,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'GINI': '1'}</t>
+          <t>{'GINI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -2054,7 +2054,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'Hobby': '1'}</t>
+          <t>{'UndergradMajor': '2', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -2070,7 +2070,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -2086,7 +2086,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Student': '1', 'Hobby': '1'}</t>
+          <t>{'HoursComputer': '2', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -2102,7 +2102,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -2118,7 +2118,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -2134,7 +2134,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -2150,7 +2150,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -2166,7 +2166,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -2182,7 +2182,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -2198,7 +2198,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'Gender': '1', 'FormalEducation': '1'}</t>
+          <t>{'Gender': '1', 'FormalEducation': '1', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -2214,7 +2214,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -2230,7 +2230,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -2246,7 +2246,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'Hobby': '1'}</t>
+          <t>{'UndergradMajor': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -2262,7 +2262,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': '2', 'Hobby': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'UndergradMajor': '2'}</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -2294,7 +2294,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -2310,7 +2310,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -2326,7 +2326,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Hobby': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -2342,7 +2342,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -2358,7 +2358,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -2374,7 +2374,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'HoursComputer': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -2406,7 +2406,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -2422,7 +2422,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -2438,7 +2438,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -2454,7 +2454,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'Hobby': '1'}</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -2470,7 +2470,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -2486,7 +2486,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -2502,7 +2502,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>{'GINI': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'GINI': '2'}</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -2518,7 +2518,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -2550,7 +2550,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -2566,7 +2566,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -2582,7 +2582,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GDP': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -2598,7 +2598,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'GINI': '2'}</t>
+          <t>{'GINI': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -2614,7 +2614,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -2630,7 +2630,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>{'Hobby': '1', 'HDI': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Hobby': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -2646,7 +2646,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -2662,7 +2662,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'HDI': '1', 'Country': '2'}</t>
+          <t>{'HDI': '1', 'Country': '2', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -2678,7 +2678,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GDP': '2', 'Country': '2'}</t>
+          <t>{'Country': '2', 'Continent': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -2694,7 +2694,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2', 'Country': '2'}</t>
+          <t>{'GINI': '2', 'Country': '2', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -2710,7 +2710,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>{'GDP': '2', 'HDI': '1', 'Country': '2'}</t>
+          <t>{'HDI': '1', 'Country': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -2742,7 +2742,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>{'GINI': '2', 'GDP': '2', 'Country': '2'}</t>
+          <t>{'GINI': '2', 'Country': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -2758,7 +2758,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'FormalEducation': '1'}</t>
+          <t>{'Gender': '1', 'FormalEducation': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -2774,7 +2774,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -2790,7 +2790,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HDI': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -2806,7 +2806,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -2822,7 +2822,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'UndergradMajor': '2'}</t>
+          <t>{'UndergradMajor': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -2838,7 +2838,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'Dependents': '2'}</t>
+          <t>{'UndergradMajor': '2', 'Dependents': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -2854,7 +2854,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'HDI': '1'}</t>
+          <t>{'UndergradMajor': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -2870,7 +2870,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -2886,7 +2886,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
+          <t>{'Student': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -2902,7 +2902,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -2918,7 +2918,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -2934,7 +2934,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HoursComputer': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -2950,7 +2950,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HoursComputer': '2'}</t>
+          <t>{'HoursComputer': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -2966,7 +2966,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HoursComputer': '2', 'HDI': '1'}</t>
+          <t>{'HoursComputer': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -2982,7 +2982,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -2998,7 +2998,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Student': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -3014,7 +3014,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -3030,7 +3030,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Student': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -3046,7 +3046,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -3062,7 +3062,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -3078,7 +3078,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GINI': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1', 'GINI': '2'}</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -3094,7 +3094,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -3110,7 +3110,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Continent': '1'}</t>
+          <t>{'SexualOrientation': '1', 'Student': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -3126,7 +3126,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -3142,7 +3142,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -3158,7 +3158,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'SexualOrientation': '1'}</t>
+          <t>{'GDP': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -3174,7 +3174,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GINI': '2', 'SexualOrientation': '1'}</t>
+          <t>{'GINI': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -3190,7 +3190,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Student': '1', 'Dependents': '2'}</t>
+          <t>{'Age': '3', 'Dependents': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -3206,7 +3206,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -3222,7 +3222,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'Student': '1', 'HDI': '1'}</t>
+          <t>{'Student': '1', 'Continent': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -3238,7 +3238,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HDI': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -3254,7 +3254,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'HDI': '1'}</t>
+          <t>{'GDP': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -3270,7 +3270,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Gender': '1', 'FormalEducation': '1'}</t>
+          <t>{'Gender': '1', 'FormalEducation': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -3286,7 +3286,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'Gender': '1', 'FormalEducation': '1'}</t>
+          <t>{'Gender': '1', 'FormalEducation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -3302,7 +3302,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1', 'FormalEducation': '1'}</t>
+          <t>{'FormalEducation': '1', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -3318,7 +3318,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -3334,7 +3334,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'UndergradMajor': '2'}</t>
+          <t>{'UndergradMajor': '2', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -3350,7 +3350,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -3366,7 +3366,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Dependents': '2'}</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -3382,7 +3382,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -3398,7 +3398,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'Dependents': '2'}</t>
+          <t>{'UndergradMajor': '2', 'Dependents': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -3414,7 +3414,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'HDI': '1'}</t>
+          <t>{'UndergradMajor': '2', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -3430,7 +3430,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': '2', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'UndergradMajor': '2', 'Dependents': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -3446,7 +3446,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -3462,7 +3462,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'DevType': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -3478,7 +3478,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -3494,7 +3494,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -3510,7 +3510,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -3526,7 +3526,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'DevType': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -3542,7 +3542,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HoursComputer': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -3558,7 +3558,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'HoursComputer': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Dependents': '2'}</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -3574,7 +3574,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -3590,7 +3590,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HoursComputer': '2', 'Dependents': '2'}</t>
+          <t>{'HoursComputer': '2', 'Dependents': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -3606,7 +3606,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HoursComputer': '2', 'HDI': '1'}</t>
+          <t>{'HoursComputer': '2', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -3622,7 +3622,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -3638,7 +3638,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -3654,7 +3654,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -3670,7 +3670,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -3686,7 +3686,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -3702,7 +3702,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GINI': '1', 'Gender': '1'}</t>
+          <t>{'GINI': '1', 'Gender': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -3718,7 +3718,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GINI': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1', 'GINI': '2'}</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -3734,7 +3734,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Age': '3', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'Dependents': '2'}</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -3750,7 +3750,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -3766,7 +3766,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -3782,7 +3782,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -3798,7 +3798,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -3814,7 +3814,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -3830,7 +3830,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>{'GINI': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'GINI': '1', 'Gender': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -3846,7 +3846,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'GINI': '1', 'Gender': '1'}</t>
+          <t>{'GINI': '1', 'Gender': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -3862,7 +3862,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'SexualOrientation': '1', 'Dependents': '2'}</t>
+          <t>{'Age': '3', 'Dependents': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -3878,7 +3878,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -3910,7 +3910,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'Continent': '1'}</t>
+          <t>{'SexualOrientation': '1', 'GDP': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -3926,7 +3926,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -3958,7 +3958,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GINI': '1', 'HDI': '1'}</t>
+          <t>{'GINI': '1', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -3974,7 +3974,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'GINI': '1'}</t>
+          <t>{'GINI': '1', 'GDP': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -3990,7 +3990,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -4006,7 +4006,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'HDI': '1', 'Continent': '1'}</t>
+          <t>{'GDP': '1', 'Continent': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -4022,7 +4022,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GDP': '2', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'Continent': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -4038,7 +4038,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2', 'HDI': '1'}</t>
+          <t>{'GINI': '2', 'HDI': '1', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -4054,7 +4054,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2', 'GDP': '2'}</t>
+          <t>{'GINI': '2', 'Continent': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -4070,7 +4070,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'GINI': '1', 'HDI': '1'}</t>
+          <t>{'GINI': '1', 'GDP': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -4086,7 +4086,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>{'GINI': '2', 'GDP': '2', 'HDI': '1'}</t>
+          <t>{'GINI': '2', 'HDI': '1', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -4102,7 +4102,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -4118,7 +4118,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'UndergradMajor': '2', 'Hobby': '1'}</t>
+          <t>{'UndergradMajor': '2', 'Hobby': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -4134,7 +4134,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'UndergradMajor': '2', 'Hobby': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -4150,7 +4150,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -4166,7 +4166,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -4182,7 +4182,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'DevType': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -4198,7 +4198,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Student': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -4214,7 +4214,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Student': '1', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'HoursComputer': '2', 'Hobby': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -4230,7 +4230,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Student': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'HoursComputer': '2', 'Hobby': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -4246,7 +4246,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -4262,7 +4262,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Student': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -4278,7 +4278,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Student': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'Hobby': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -4294,7 +4294,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -4310,7 +4310,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -4326,7 +4326,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'Hobby': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -4342,7 +4342,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -4358,7 +4358,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Hobby': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -4374,7 +4374,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'Student': '1', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -4390,7 +4390,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B243" t="n">
@@ -4406,7 +4406,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'UndergradMajor': '2', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Hobby': '1', 'Dependents': '2'}</t>
         </is>
       </c>
       <c r="B244" t="n">
@@ -4422,7 +4422,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': '2', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Hobby': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B245" t="n">
@@ -4438,7 +4438,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'UndergradMajor': '2', 'Hobby': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -4454,7 +4454,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -4470,7 +4470,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'DevType': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -4486,7 +4486,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -4502,7 +4502,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -4518,7 +4518,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Hobby': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B251" t="n">
@@ -4534,7 +4534,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'HoursComputer': '2', 'Hobby': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B252" t="n">
@@ -4550,7 +4550,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -4566,7 +4566,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B254" t="n">
@@ -4582,7 +4582,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'Hobby': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B255" t="n">
@@ -4598,7 +4598,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B256" t="n">
@@ -4614,7 +4614,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'Hobby': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'SexualOrientation': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B257" t="n">
@@ -4630,7 +4630,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'GINI': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'SexualOrientation': '1', 'GINI': '2'}</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -4646,7 +4646,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'Hobby': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B259" t="n">
@@ -4662,7 +4662,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Hobby': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Hobby': '1', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B260" t="n">
@@ -4678,7 +4678,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Hobby': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B261" t="n">
@@ -4694,7 +4694,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GDP': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'Hobby': '1', 'SexualOrientation': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B262" t="n">
@@ -4710,7 +4710,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GDP': '2', 'HDI': '1', 'Country': '2'}</t>
+          <t>{'HDI': '1', 'Country': '2', 'Continent': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B263" t="n">
@@ -4726,7 +4726,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2', 'HDI': '1', 'Country': '2'}</t>
+          <t>{'GINI': '2', 'HDI': '1', 'Country': '2', 'Continent': '2'}</t>
         </is>
       </c>
       <c r="B264" t="n">
@@ -4742,7 +4742,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2', 'GDP': '2', 'Country': '2'}</t>
+          <t>{'GINI': '2', 'Country': '2', 'Continent': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B265" t="n">
@@ -4758,7 +4758,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>{'GINI': '2', 'GDP': '2', 'HDI': '1', 'Country': '2'}</t>
+          <t>{'GINI': '2', 'HDI': '1', 'Country': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B266" t="n">
@@ -4774,7 +4774,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Gender': '1', 'FormalEducation': '1'}</t>
+          <t>{'Gender': '1', 'FormalEducation': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B267" t="n">
@@ -4790,7 +4790,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B268" t="n">
@@ -4806,7 +4806,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'UndergradMajor': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B269" t="n">
@@ -4822,7 +4822,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'UndergradMajor': '2', 'HDI': '1'}</t>
+          <t>{'UndergradMajor': '2', 'HDI': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B270" t="n">
@@ -4838,7 +4838,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B271" t="n">
@@ -4854,7 +4854,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'Student': '1', 'DevType': '2'}</t>
         </is>
       </c>
       <c r="B272" t="n">
@@ -4870,7 +4870,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'Student': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'HDI': '1', 'Student': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B273" t="n">
@@ -4886,7 +4886,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HoursComputer': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B274" t="n">
@@ -4902,7 +4902,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HoursComputer': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B275" t="n">
@@ -4918,7 +4918,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HoursComputer': '2', 'HDI': '1'}</t>
+          <t>{'HoursComputer': '2', 'HDI': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B276" t="n">
@@ -4934,7 +4934,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Student': '1', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B277" t="n">
@@ -4950,7 +4950,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1', 'Student': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B278" t="n">
@@ -4966,7 +4966,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Student': '1', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B279" t="n">
@@ -4982,7 +4982,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B280" t="n">
@@ -4998,7 +4998,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'Student': '1', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B281" t="n">
@@ -5014,7 +5014,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GINI': '2', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Student': '1', 'SexualOrientation': '1', 'GINI': '2'}</t>
         </is>
       </c>
       <c r="B282" t="n">
@@ -5030,7 +5030,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'Student': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B283" t="n">
@@ -5046,7 +5046,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'Student': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B284" t="n">
@@ -5062,7 +5062,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B285" t="n">
@@ -5078,7 +5078,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HDI': '1', 'Dependents': '2'}</t>
+          <t>{'Dependents': '2', 'Student': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B286" t="n">
@@ -5094,7 +5094,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'HDI': '1', 'Age': '3'}</t>
+          <t>{'Age': '3', 'HDI': '1', 'Student': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B287" t="n">
@@ -5110,7 +5110,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'GDP': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'GDP': '1', 'Student': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B288" t="n">
@@ -5126,7 +5126,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1', 'Gender': '1', 'FormalEducation': '1'}</t>
+          <t>{'Gender': '1', 'FormalEducation': '1', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B289" t="n">
@@ -5142,7 +5142,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B290" t="n">
@@ -5158,7 +5158,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'SexualOrientation': '1', 'UndergradMajor': '2', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Dependents': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B291" t="n">
@@ -5174,7 +5174,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'UndergradMajor': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B292" t="n">
@@ -5190,7 +5190,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'UndergradMajor': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'UndergradMajor': '2', 'Dependents': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B293" t="n">
@@ -5206,7 +5206,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'DevType': '2', 'SexualOrientation': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B294" t="n">
@@ -5222,7 +5222,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>{'DevType': '2', 'SexualOrientation': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HDI': '1', 'DevType': '2', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B295" t="n">
@@ -5238,7 +5238,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HoursComputer': '2', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'HoursComputer': '2', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B296" t="n">
@@ -5254,7 +5254,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>{'Dependents': '2', 'SexualOrientation': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Dependents': '2', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B297" t="n">
@@ -5270,7 +5270,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'HDI': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1', 'HDI': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B298" t="n">
@@ -5286,7 +5286,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'SexualOrientation': '1', 'GDP': '1', 'Continent': '1'}</t>
         </is>
       </c>
       <c r="B299" t="n">
@@ -5302,7 +5302,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>{'Age': '3', 'SexualOrientation': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'Age': '3', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B300" t="n">
@@ -5318,7 +5318,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B301" t="n">
@@ -5334,7 +5334,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': '1', 'GINI': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'GINI': '1', 'Gender': '1', 'HDI': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B302" t="n">
@@ -5350,7 +5350,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'SexualOrientation': '1', 'GINI': '1', 'Gender': '1'}</t>
+          <t>{'GINI': '1', 'Gender': '1', 'GDP': '1', 'SexualOrientation': '1'}</t>
         </is>
       </c>
       <c r="B303" t="n">
@@ -5366,7 +5366,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'HDI': '1', 'Continent': '1', 'Gender': '1'}</t>
+          <t>{'Gender': '1', 'GDP': '1', 'Continent': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B304" t="n">
@@ -5382,7 +5382,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>{'GDP': '1', 'GINI': '1', 'HDI': '1', 'Gender': '1'}</t>
+          <t>{'GINI': '1', 'Gender': '1', 'GDP': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B305" t="n">
@@ -5398,7 +5398,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'GDP': '1', 'SexualOrientation': '1', 'Continent': '1'}</t>
+          <t>{'SexualOrientation': '1', 'GDP': '1', 'Continent': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B306" t="n">
@@ -5414,7 +5414,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>{'HDI': '1', 'GDP': '1', 'SexualOrientation': '1', 'GINI': '1'}</t>
+          <t>{'GINI': '1', 'GDP': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B307" t="n">
@@ -5430,7 +5430,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>{'Continent': '2', 'GINI': '2', 'GDP': '2', 'HDI': '1'}</t>
+          <t>{'GINI': '2', 'HDI': '1', 'Continent': '2', 'GDP': '2'}</t>
         </is>
       </c>
       <c r="B308" t="n">
@@ -5446,7 +5446,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'UndergradMajor': '2'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'UndergradMajor': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B309" t="n">
@@ -5462,7 +5462,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'Hobby': '1', 'HDI': '1', 'UndergradMajor': '2'}</t>
+          <t>{'Hobby': '1', 'Gender': '1', 'UndergradMajor': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B310" t="n">
@@ -5478,7 +5478,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'UndergradMajor': '2'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'UndergradMajor': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B311" t="n">
@@ -5494,7 +5494,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'DevType': '2'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'SexualOrientation': '1', 'Gender': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B312" t="n">
@@ -5510,7 +5510,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'Hobby': '1', 'HDI': '1', 'DevType': '2'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'Gender': '1', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B313" t="n">
@@ -5526,7 +5526,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'DevType': '2'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'SexualOrientation': '1', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B314" t="n">
@@ -5542,7 +5542,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HoursComputer': '2', 'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'HoursComputer': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B315" t="n">
@@ -5558,7 +5558,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'Dependents': '2', 'SexualOrientation': '1', 'Hobby': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'Dependents': '2', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B316" t="n">
@@ -5574,7 +5574,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B317" t="n">
@@ -5590,7 +5590,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'Dependents': '2', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'Gender': '1', 'Dependents': '2', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B318" t="n">
@@ -5606,7 +5606,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Dependents': '2', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Dependents': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B319" t="n">
@@ -5622,7 +5622,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>{'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'UndergradMajor': '2'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'UndergradMajor': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B320" t="n">
@@ -5638,7 +5638,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>{'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'DevType': '2'}</t>
+          <t>{'Hobby': '1', 'DevType': '2', 'SexualOrientation': '1', 'Gender': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B321" t="n">
@@ -5654,7 +5654,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>{'HoursComputer': '2', 'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'HoursComputer': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B322" t="n">
@@ -5670,7 +5670,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>{'Gender': '1', 'Dependents': '2', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'Dependents': '2', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B323" t="n">
@@ -5686,7 +5686,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>{'Gender': '1', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1', 'GDP': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B324" t="n">
@@ -5702,7 +5702,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>{'GINI': '2', 'GDP': '2', 'Continent': '2', 'HDI': '1', 'Country': '2'}</t>
+          <t>{'Continent': '2', 'HDI': '1', 'GDP': '2', 'GINI': '2', 'Country': '2'}</t>
         </is>
       </c>
       <c r="B325" t="n">
@@ -5718,7 +5718,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'SexualOrientation': '1', 'HDI': '1', 'UndergradMajor': '2'}</t>
+          <t>{'SexualOrientation': '1', 'Gender': '1', 'UndergradMajor': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B326" t="n">
@@ -5734,7 +5734,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'SexualOrientation': '1', 'HDI': '1', 'DevType': '2'}</t>
+          <t>{'DevType': '2', 'SexualOrientation': '1', 'Gender': '1', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B327" t="n">
@@ -5750,7 +5750,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'HoursComputer': '2', 'Gender': '1', 'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'SexualOrientation': '1', 'Gender': '1', 'HoursComputer': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B328" t="n">
@@ -5766,7 +5766,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'Dependents': '2', 'SexualOrientation': '1', 'HDI': '1'}</t>
+          <t>{'SexualOrientation': '1', 'Gender': '1', 'Dependents': '2', 'Student': '1', 'HDI': '1'}</t>
         </is>
       </c>
       <c r="B329" t="n">
@@ -5782,7 +5782,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'SexualOrientation': '1', 'HDI': '1', 'GDP': '1'}</t>
+          <t>{'SexualOrientation': '1', 'Gender': '1', 'HDI': '1', 'Student': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B330" t="n">
@@ -5798,7 +5798,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>{'Gender': '1', 'SexualOrientation': '1', 'HDI': '1', 'Continent': '1', 'GDP': '1'}</t>
+          <t>{'SexualOrientation': '1', 'Gender': '1', 'Continent': '1', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B331" t="n">
@@ -5814,7 +5814,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>{'Gender': '1', 'GDP': '1', 'SexualOrientation': '1', 'HDI': '1', 'GINI': '1'}</t>
+          <t>{'SexualOrientation': '1', 'GINI': '1', 'Gender': '1', 'HDI': '1', 'GDP': '1'}</t>
         </is>
       </c>
       <c r="B332" t="n">
@@ -5830,7 +5830,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>{'Student': '1', 'Gender': '1', 'Dependents': '2', 'SexualOrientation': '1', 'Hobby': '1', 'HDI': '1'}</t>
+          <t>{'Hobby': '1', 'SexualOrientation': '1', 'Gender': '1', 'Dependents': '2', 'HDI': '1', 'Student': '1'}</t>
         </is>
       </c>
       <c r="B333" t="n">

</xml_diff>